<commit_message>
feat: adjust table cells for better readability
</commit_message>
<xml_diff>
--- a/ITSC 3155 User Stories.xlsx
+++ b/ITSC 3155 User Stories.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Montay\OneDrive\Documents\ITSC 3155\Restaurant-API\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E95EC5E-693A-41FE-BAA2-96DA1CD5CD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -259,50 +268,56 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF2F75B5"/>
       <name val="Century Gothic"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;⋎ntury Gothic\&quot;&quot;"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
     </font>
@@ -312,7 +327,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -340,27 +355,39 @@
     </fill>
   </fills>
   <borders count="7">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -370,6 +397,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -378,19 +406,25 @@
       <right style="thin">
         <color rgb="FFBFBFBF"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FFBFBFBF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FFBFBFBF"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FFBFBFBF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FFBFBFBF"/>
       </right>
@@ -400,95 +434,97 @@
       <bottom style="thin">
         <color rgb="FFBFBFBF"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -678,679 +714,691 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.63"/>
-    <col customWidth="1" min="2" max="3" width="31.5"/>
-    <col customWidth="1" min="4" max="4" width="34.13"/>
-    <col customWidth="1" min="5" max="5" width="33.63"/>
-    <col customWidth="1" min="6" max="6" width="31.38"/>
-    <col customWidth="1" min="8" max="8" width="14.63"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="1:8" ht="67.5">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="13">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="H4" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="54">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="13">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="H5" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="54">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="13">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="H6" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="40.5">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="13">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="H7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="54">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="18">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="H8" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="54">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="18">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="14">
-        <v>7.0</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="H9" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="54">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="18">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="14">
-        <v>8.0</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="H10" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="54">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="18">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="14">
-        <v>9.0</v>
-      </c>
-      <c r="B12" s="15" t="s">
+      <c r="H11" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="54">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="18">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="14">
-        <v>10.0</v>
-      </c>
-      <c r="B13" s="15" t="s">
+      <c r="H12" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="54">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="18">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="14">
-        <v>11.0</v>
-      </c>
-      <c r="B14" s="15" t="s">
+      <c r="H13" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="54">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="18">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="14">
-        <v>12.0</v>
-      </c>
-      <c r="B15" s="15" t="s">
+      <c r="H14" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="54">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="18">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="14">
-        <v>13.0</v>
-      </c>
-      <c r="B16" s="15" t="s">
+      <c r="H15" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="54">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="18">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="14">
-        <v>14.0</v>
-      </c>
-      <c r="B17" s="15" t="s">
+      <c r="H16" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="54">
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="18">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="19">
-        <v>15.0</v>
-      </c>
-      <c r="B18" s="20" t="s">
+      <c r="H17" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="54">
+      <c r="A18" s="14">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="21">
-        <v>3.0</v>
-      </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="19">
-        <v>16.0</v>
-      </c>
-      <c r="B19" s="20" t="s">
+      <c r="H18" s="16">
+        <v>3</v>
+      </c>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+    </row>
+    <row r="19" spans="1:12" ht="67.5">
+      <c r="A19" s="14">
+        <v>16</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="21">
-        <v>2.0</v>
-      </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23" t="s">
+      <c r="H19" s="16">
+        <v>2</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+    </row>
+    <row r="20" spans="1:12" ht="27">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="24">
-        <v>59.0</v>
-      </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
+      <c r="H20" s="19">
+        <v>59</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
     </row>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
@@ -2324,11 +2372,11 @@
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G19">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G19" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>